<commit_message>
changement police de caractere switch small
</commit_message>
<xml_diff>
--- a/2_Strategie/switchs2017excel.xlsx
+++ b/2_Strategie/switchs2017excel.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen_000\Desktop\ESEO\robotSVN\robot_eseo\2_Strategie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ClubRobot\CodeSource\2_Strategie\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4032"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -83,18 +83,6 @@
     <t>RETURN_ADV_SIDE</t>
   </si>
   <si>
-    <t>ANNE_RETURN_MIDDLE</t>
-  </si>
-  <si>
-    <t>RETURN_ADV_MIDDLE</t>
-  </si>
-  <si>
-    <t>TAKE_OUR_ROCKET</t>
-  </si>
-  <si>
-    <t>TAKE_ADV_ROCKET</t>
-  </si>
-  <si>
     <t>DISPOSE_MIDDLE</t>
   </si>
   <si>
@@ -123,13 +111,25 @@
   </si>
   <si>
     <t>ACT_MAGIC_ARM</t>
+  </si>
+  <si>
+    <t>OUR_ROCKET</t>
+  </si>
+  <si>
+    <t>ADV_ROCKET</t>
+  </si>
+  <si>
+    <t>RETURN_MIDDLE</t>
+  </si>
+  <si>
+    <t>RET_ADV_MIDDLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +147,22 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -280,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -327,6 +343,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,7 +367,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -609,24 +631,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="0.85546875" customWidth="1"/>
-    <col min="2" max="3" width="2.28515625" customWidth="1"/>
-    <col min="4" max="4" width="0.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" customWidth="1"/>
-    <col min="7" max="7" width="0.85546875" customWidth="1"/>
-    <col min="8" max="9" width="2.28515625" customWidth="1"/>
-    <col min="10" max="10" width="0.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="0.88671875" customWidth="1"/>
+    <col min="2" max="3" width="2.33203125" customWidth="1"/>
+    <col min="4" max="4" width="0.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" customWidth="1"/>
+    <col min="7" max="7" width="0.88671875" customWidth="1"/>
+    <col min="8" max="9" width="2.33203125" customWidth="1"/>
+    <col min="10" max="10" width="0.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
         <v>16</v>
       </c>
@@ -634,7 +656,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -646,7 +668,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="12" t="s">
         <v>14</v>
@@ -665,9 +687,9 @@
         <v>15</v>
       </c>
       <c r="J4" s="14"/>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -678,9 +700,9 @@
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
       <c r="J5" s="14"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="12" t="s">
         <v>14</v>
@@ -699,11 +721,11 @@
         <v>15</v>
       </c>
       <c r="J6" s="14"/>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -714,9 +736,9 @@
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="12" t="s">
         <v>14</v>
@@ -741,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -752,9 +774,9 @@
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
       <c r="J9" s="14"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="12" t="s">
         <v>14</v>
@@ -773,11 +795,11 @@
         <v>15</v>
       </c>
       <c r="J10" s="14"/>
-      <c r="K10" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -788,9 +810,9 @@
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="12" t="s">
         <v>14</v>
@@ -809,11 +831,11 @@
         <v>15</v>
       </c>
       <c r="J12" s="14"/>
-      <c r="K12" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -824,9 +846,9 @@
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="14"/>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="13" t="s">
         <v>14</v>
@@ -847,11 +869,11 @@
         <v>15</v>
       </c>
       <c r="J14" s="14"/>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="26" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -862,9 +884,9 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
       <c r="J15" s="14"/>
-      <c r="K15" s="8"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="12" t="s">
         <v>14</v>
@@ -886,10 +908,10 @@
       </c>
       <c r="J16" s="14"/>
       <c r="K16" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -900,9 +922,9 @@
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
       <c r="J17" s="14"/>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="12" t="s">
         <v>14</v>
@@ -924,10 +946,10 @@
       </c>
       <c r="J18" s="14"/>
       <c r="K18" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -940,7 +962,7 @@
       <c r="J19" s="19"/>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
       <c r="D20" s="22"/>
@@ -952,7 +974,7 @@
       <c r="J20" s="22"/>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="23"/>
       <c r="C21" s="23"/>
@@ -965,7 +987,7 @@
       <c r="J21" s="24"/>
       <c r="K21" s="11"/>
     </row>
-    <row r="22" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="12" t="s">
         <v>14</v>
@@ -986,11 +1008,11 @@
         <v>15</v>
       </c>
       <c r="J22" s="14"/>
-      <c r="K22" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1001,9 +1023,9 @@
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
       <c r="J23" s="14"/>
-      <c r="K23" s="8"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="27"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="12" t="s">
         <v>14</v>
@@ -1024,11 +1046,11 @@
         <v>15</v>
       </c>
       <c r="J24" s="14"/>
-      <c r="K24" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -1039,9 +1061,9 @@
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
       <c r="J25" s="14"/>
-      <c r="K25" s="8"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="27"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="12" t="s">
         <v>14</v>
@@ -1062,11 +1084,11 @@
         <v>15</v>
       </c>
       <c r="J26" s="14"/>
-      <c r="K26" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -1077,9 +1099,9 @@
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="14"/>
-      <c r="K27" s="8"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="27"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="12" t="s">
         <v>14</v>
@@ -1100,11 +1122,11 @@
         <v>15</v>
       </c>
       <c r="J28" s="14"/>
-      <c r="K28" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -1115,9 +1137,9 @@
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
       <c r="J29" s="14"/>
-      <c r="K29" s="8"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="27"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="12" t="s">
         <v>14</v>
@@ -1138,11 +1160,11 @@
         <v>15</v>
       </c>
       <c r="J30" s="14"/>
-      <c r="K30" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -1155,7 +1177,7 @@
       <c r="J31" s="19"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
       <c r="D32" s="22"/>
@@ -1167,7 +1189,7 @@
       <c r="J32" s="22"/>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="23"/>
       <c r="C33" s="23"/>
@@ -1180,7 +1202,7 @@
       <c r="J33" s="24"/>
       <c r="K33" s="11"/>
     </row>
-    <row r="34" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="12" t="s">
         <v>14</v>
@@ -1202,10 +1224,10 @@
       </c>
       <c r="J34" s="14"/>
       <c r="K34" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -1218,7 +1240,7 @@
       <c r="J35" s="14"/>
       <c r="K35" s="8"/>
     </row>
-    <row r="36" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="12" t="s">
         <v>14</v>
@@ -1238,10 +1260,10 @@
       </c>
       <c r="J36" s="14"/>
       <c r="K36" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -1254,7 +1276,7 @@
       <c r="J37" s="14"/>
       <c r="K37" s="8"/>
     </row>
-    <row r="38" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="13" t="s">
         <v>15</v>
@@ -1275,11 +1297,11 @@
         <v>14</v>
       </c>
       <c r="J38" s="14"/>
-      <c r="K38" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -1292,7 +1314,7 @@
       <c r="J39" s="14"/>
       <c r="K39" s="8"/>
     </row>
-    <row r="40" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="13" t="s">
         <v>15</v>
@@ -1314,10 +1336,10 @@
       </c>
       <c r="J40" s="14"/>
       <c r="K40" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -1330,7 +1352,7 @@
       <c r="J41" s="14"/>
       <c r="K41" s="8"/>
     </row>
-    <row r="42" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="13" t="s">
         <v>15</v>
@@ -1352,10 +1374,10 @@
       </c>
       <c r="J42" s="14"/>
       <c r="K42" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -1368,7 +1390,7 @@
       <c r="J43" s="14"/>
       <c r="K43" s="8"/>
     </row>
-    <row r="44" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="13" t="s">
         <v>15</v>
@@ -1393,7 +1415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1405,19 +1427,19 @@
       <c r="J45" s="6"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>